<commit_message>
DCF for TJX Companies (TJX)
Created DCF for TJX Companies (TJX), 9Q, 5Y
Revised BBBY model
Added notes to ATKR and WIRE
</commit_message>
<xml_diff>
--- a/Models/ATKR.xlsx
+++ b/Models/ATKR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FFCCAC-F241-4797-9651-04F3CC25FB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DBFCD7-CBE0-4140-A700-25B41D698275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28260" yWindow="3780" windowWidth="15825" windowHeight="17250" xr2:uid="{2EC0F4CB-CC56-4207-8108-7C832533A8D8}"/>
+    <workbookView xWindow="3690" yWindow="1350" windowWidth="19005" windowHeight="13650" xr2:uid="{2EC0F4CB-CC56-4207-8108-7C832533A8D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
   <si>
     <t>Atkore </t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>Target</t>
+  </si>
+  <si>
+    <t>2022 climate legislation also boosts potential tax credits for construction of some EV charging stations to as much as $100,000 per charger, up from $30,000 per site currently</t>
   </si>
 </sst>
 </file>
@@ -772,7 +775,7 @@
   <dimension ref="B1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,6 +850,9 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
       <c r="M8" t="s">
         <v>12</v>
       </c>

</xml_diff>